<commit_message>
09-05-2023 financial statment continue... added ratio and others
</commit_message>
<xml_diff>
--- a/financial_knwoledge/financial_statment.xlsx
+++ b/financial_knwoledge/financial_statment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7890" windowHeight="6030" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7890" windowHeight="6030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="financial statment" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="173">
   <si>
     <t>Financial statement</t>
   </si>
@@ -132,9 +132,6 @@
     <t>summary, accrued expenses are expenses that have been incurred but not yet paid, and they are recognized as a liability on the balance sheet until they are paid.</t>
   </si>
   <si>
-    <t>Short tem notes paybale</t>
-  </si>
-  <si>
     <t>Short-term notes payable are a type of debt that a company owes to creditors or lenders that is due within one year or less</t>
   </si>
   <si>
@@ -168,12 +165,6 @@
     <t>Debt-to-Equity Ratio</t>
   </si>
   <si>
-    <t>Return on Equity</t>
-  </si>
-  <si>
-    <t>Gross Margin Ratio</t>
-  </si>
-  <si>
     <t>Inventory Turnover Ratio</t>
   </si>
   <si>
@@ -186,12 +177,6 @@
     <t>This ratio measures the profitability of a company's equity investment</t>
   </si>
   <si>
-    <t>This ratio measures the profitability of a company's sales</t>
-  </si>
-  <si>
-    <t>dividing gross profit by sales revenue</t>
-  </si>
-  <si>
     <t>his ratio measures the efficiency of a company's inventory management</t>
   </si>
   <si>
@@ -315,9 +300,6 @@
     <t>The income statement, also known as the profit and loss statement, is a financial statement that summarizes a company's revenues, expenses, and net income over a specific period of time. It provides an overview of a company's financial performance during the period and is an important tool for investors, creditors, and other stakeholders to assess the company's profitability</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales revenue</t>
   </si>
   <si>
@@ -339,9 +321,6 @@
     <t>Less:Ending inventory</t>
   </si>
   <si>
-    <t>Cost of good sold</t>
-  </si>
-  <si>
     <t>Operating expenses:</t>
   </si>
   <si>
@@ -357,12 +336,6 @@
     <t>Other income and expenses:</t>
   </si>
   <si>
-    <t>interset income</t>
-  </si>
-  <si>
-    <t>interset expense</t>
-  </si>
-  <si>
     <t xml:space="preserve">Other income </t>
   </si>
   <si>
@@ -405,9 +378,6 @@
     <t>Operating Profit Margin = Operating Income / Sales Revenue</t>
   </si>
   <si>
-    <t>Net profit margin:</t>
-  </si>
-  <si>
     <t>This ratio measures the percentage of sales revenue that remains after deducting all expenses, including taxes and interest. It is calculated by dividing net income by sales revenue.</t>
   </si>
   <si>
@@ -487,6 +457,96 @@
   </si>
   <si>
     <t>Cash and cash equivalents, end of year</t>
+  </si>
+  <si>
+    <t>Sales returns and allowances are a common accounting concept that refers to the reduction in revenue that occurs when a customer returns a product or receives a discount due to an issue with the product or service provided</t>
+  </si>
+  <si>
+    <t>Beginning inventory is the value of a company's inventory at the beginning of an accounting period. It represents the inventory that was carried over from the previous accounting period and is the starting point for determining the cost of goods sold and ending inventory for the current period.</t>
+  </si>
+  <si>
+    <t>Ending inventory is the value of a company's inventory at the end of an accounting period. It represents the value of the inventory that was not sold or used during the period and is the starting point for determining the cost of goods sold for the next accounting period</t>
+  </si>
+  <si>
+    <t>Purchase refers to the acquisition of goods or services by a business from a supplier or vendor. Purchases are an essential part of a company's operations and are necessary for producing and selling products or providing services</t>
+  </si>
+  <si>
+    <t>Cost of goods sold (COGS) is the direct cost of producing or purchasing the products or services that a company sells during a specific accounting period. COGS is an important financial metric used in accounting and financial analysis as it directly impacts a company's gross profit and net income</t>
+  </si>
+  <si>
+    <t>COGS includes the cost of the raw materials or goods used in production, the direct labor costs associated with producing the goods or services, and any overhead costs directly related to production. Indirect costs, such as administrative and marketing expenses, are not included in COGS</t>
+  </si>
+  <si>
+    <t>Operating expenses, also known as OPEX, are the costs associated with running a business's day-to-day operations. These expenses are distinct from the cost of goods sold (COGS) and are typically categorized as selling, general, and administrative (SG&amp;A) expenses on a company's income statement</t>
+  </si>
+  <si>
+    <t>Examples of operating expenses include salaries and wages, rent, utilities, insurance, advertising and marketing expenses, legal fees, office supplies, and maintenance expenses</t>
+  </si>
+  <si>
+    <t>Selling expenses are a type of operating expense that are directly related to the marketing and sale of a company's products or services.</t>
+  </si>
+  <si>
+    <t>Advertising and promotion costs:,Sales commissions:,Shipping and delivery costs,Sales salaries and wages,Trade show expenses</t>
+  </si>
+  <si>
+    <t>the costs associated with the day-to-day management and administration of a company. These expenses are not directly related to the production or sale of a company's products or services, but are necessary for the overall operation of the business.</t>
+  </si>
+  <si>
+    <t>Salaries and wages,Rent and utilities,Office supplies,Legal and professional fees,Insurance,Depreciation and amortization</t>
+  </si>
+  <si>
+    <t>interest income</t>
+  </si>
+  <si>
+    <t>interest expense</t>
+  </si>
+  <si>
+    <t>Interest income is the income earned by an individual or a business from investments or deposits that earn interest.</t>
+  </si>
+  <si>
+    <t>Interest earned on savings accounts,Interest earned on certificates of deposit,Interest earned on bonds,Interest earned on loans:,Interest earned on cash equivalents</t>
+  </si>
+  <si>
+    <t>nterest expense is the cost that an individual or business incurs on borrowed money. It represents the amount of interest that must be paid on loans or other credit facilities</t>
+  </si>
+  <si>
+    <t>Interest paid on mortgages,Interest paid on loans,Interest paid on credit cards,Interest paid on bonds</t>
+  </si>
+  <si>
+    <t>EXPENSES</t>
+  </si>
+  <si>
+    <t>PROFITS</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>$Cost of good sold</t>
+  </si>
+  <si>
+    <t>Price-Earnings Ratio(P/E)</t>
+  </si>
+  <si>
+    <t>P/E ratio = Current stock price / EPS</t>
+  </si>
+  <si>
+    <t>Times Interest Earned(interest coverage ratio)</t>
+  </si>
+  <si>
+    <t>TIE = EBIT / Interest expense</t>
+  </si>
+  <si>
+    <t>Times interest earned (TIE), also known as interest coverage ratio, is a financial ratio that measures a company's ability to meet its interest obligations on its debt</t>
+  </si>
+  <si>
+    <t>Return on Equity(ROE)</t>
+  </si>
+  <si>
+    <t>Net profit margin</t>
+  </si>
+  <si>
+    <t>Short term notes paybale</t>
   </si>
 </sst>
 </file>
@@ -496,7 +556,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +623,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF343541"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -581,11 +647,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -613,10 +680,14 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -932,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ162"/>
+  <dimension ref="A1:AJ159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +1019,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -997,7 +1068,7 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1426,7 +1497,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1551,14 +1622,14 @@
     </row>
     <row r="15" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="B15" s="4">
         <v>30000</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1602,7 +1673,7 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1763,7 +1834,7 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1807,7 +1878,7 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1851,7 +1922,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2088,12 +2159,12 @@
     </row>
     <row r="28" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2168,7 +2239,7 @@
     </row>
     <row r="30" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2208,18 +2279,21 @@
     </row>
     <row r="31" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="B31" s="17">
+        <f>+(B3+B4+B5+B6)/(B14+B13+B15)</f>
+        <v>2.9090909090909092</v>
+      </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -2254,18 +2328,21 @@
     </row>
     <row r="32" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="B32" s="17">
+        <f>+(B3+B4+B6-B5)/(B13+B14+B15)</f>
+        <v>0.18181818181818182</v>
+      </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -2300,18 +2377,21 @@
     </row>
     <row r="33" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="B33" s="17">
+        <f>+(B16+B15)/B23</f>
+        <v>0.83870967741935487</v>
+      </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -2346,17 +2426,19 @@
     </row>
     <row r="34" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -2390,15 +2472,15 @@
     </row>
     <row r="35" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -2433,17 +2515,11 @@
       <c r="AJ35" s="4"/>
     </row>
     <row r="36" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -2478,19 +2554,17 @@
     </row>
     <row r="37" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -2524,17 +2598,19 @@
     </row>
     <row r="38" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -2605,17 +2681,11 @@
       <c r="AJ39" s="4"/>
     </row>
     <row r="40" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -2649,20 +2719,12 @@
       <c r="AJ40" s="4"/>
     </row>
     <row r="41" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
@@ -7178,120 +7240,6 @@
       <c r="AI159" s="4"/>
       <c r="AJ159" s="4"/>
     </row>
-    <row r="160" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A160" s="4"/>
-      <c r="B160" s="4"/>
-      <c r="C160" s="4"/>
-      <c r="D160" s="4"/>
-      <c r="E160" s="4"/>
-      <c r="F160" s="4"/>
-      <c r="G160" s="4"/>
-      <c r="H160" s="4"/>
-      <c r="I160" s="4"/>
-      <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
-      <c r="L160" s="4"/>
-      <c r="M160" s="4"/>
-      <c r="N160" s="4"/>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
-      <c r="Q160" s="4"/>
-      <c r="R160" s="4"/>
-      <c r="S160" s="4"/>
-      <c r="T160" s="4"/>
-      <c r="U160" s="4"/>
-      <c r="V160" s="4"/>
-      <c r="W160" s="4"/>
-      <c r="X160" s="4"/>
-      <c r="Y160" s="4"/>
-      <c r="Z160" s="4"/>
-      <c r="AA160" s="4"/>
-      <c r="AB160" s="4"/>
-      <c r="AC160" s="4"/>
-      <c r="AD160" s="4"/>
-      <c r="AE160" s="4"/>
-      <c r="AF160" s="4"/>
-      <c r="AG160" s="4"/>
-      <c r="AH160" s="4"/>
-      <c r="AI160" s="4"/>
-      <c r="AJ160" s="4"/>
-    </row>
-    <row r="161" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A161" s="4"/>
-      <c r="B161" s="4"/>
-      <c r="C161" s="4"/>
-      <c r="D161" s="4"/>
-      <c r="E161" s="4"/>
-      <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
-      <c r="H161" s="4"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
-      <c r="L161" s="4"/>
-      <c r="M161" s="4"/>
-      <c r="N161" s="4"/>
-      <c r="O161" s="4"/>
-      <c r="P161" s="4"/>
-      <c r="Q161" s="4"/>
-      <c r="R161" s="4"/>
-      <c r="S161" s="4"/>
-      <c r="T161" s="4"/>
-      <c r="U161" s="4"/>
-      <c r="V161" s="4"/>
-      <c r="W161" s="4"/>
-      <c r="X161" s="4"/>
-      <c r="Y161" s="4"/>
-      <c r="Z161" s="4"/>
-      <c r="AA161" s="4"/>
-      <c r="AB161" s="4"/>
-      <c r="AC161" s="4"/>
-      <c r="AD161" s="4"/>
-      <c r="AE161" s="4"/>
-      <c r="AF161" s="4"/>
-      <c r="AG161" s="4"/>
-      <c r="AH161" s="4"/>
-      <c r="AI161" s="4"/>
-      <c r="AJ161" s="4"/>
-    </row>
-    <row r="162" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A162" s="4"/>
-      <c r="B162" s="4"/>
-      <c r="C162" s="4"/>
-      <c r="D162" s="4"/>
-      <c r="E162" s="4"/>
-      <c r="F162" s="4"/>
-      <c r="G162" s="4"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
-      <c r="N162" s="4"/>
-      <c r="O162" s="4"/>
-      <c r="P162" s="4"/>
-      <c r="Q162" s="4"/>
-      <c r="R162" s="4"/>
-      <c r="S162" s="4"/>
-      <c r="T162" s="4"/>
-      <c r="U162" s="4"/>
-      <c r="V162" s="4"/>
-      <c r="W162" s="4"/>
-      <c r="X162" s="4"/>
-      <c r="Y162" s="4"/>
-      <c r="Z162" s="4"/>
-      <c r="AA162" s="4"/>
-      <c r="AB162" s="4"/>
-      <c r="AC162" s="4"/>
-      <c r="AD162" s="4"/>
-      <c r="AE162" s="4"/>
-      <c r="AF162" s="4"/>
-      <c r="AG162" s="4"/>
-      <c r="AH162" s="4"/>
-      <c r="AI162" s="4"/>
-      <c r="AJ162" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7300,10 +7248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7316,7 +7264,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>11</v>
@@ -7334,17 +7282,17 @@
     </row>
     <row r="3" spans="1:5" ht="120.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>95</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1">
         <v>500000</v>
@@ -7352,224 +7300,422 @@
     </row>
     <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1">
         <v>-10000</v>
       </c>
+      <c r="D7" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1">
         <f>+SUM(B6:B7)</f>
         <v>490000</v>
       </c>
     </row>
+    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+    </row>
     <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="1">
-        <v>50000</v>
+      <c r="A11" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1">
-        <v>200000</v>
+        <v>50000</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1">
-        <v>-60000</v>
+        <v>200000</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-60000</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="1">
+        <f>+SUM(B12:B14)</f>
+        <v>190000</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1">
+        <f>+B8-B15</f>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="1">
+        <v>75000</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="1">
+        <f>+SUM(B20:B21)</f>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-10000</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="1">
+        <f>+SUM(B26:B28)</f>
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="1">
+        <f>+B17-B22+B29</f>
+        <v>173000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="1">
-        <f>+SUM(B11:B13)</f>
-        <v>190000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="B32" s="1">
+        <v>-40000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="1">
+        <f>+SUM(B31:B32)</f>
+        <v>133000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="15">
+        <f>+(B6-B15)/B6</f>
+        <v>0.62</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="15">
+        <f>+B22/B6</f>
+        <v>0.25</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="1">
-        <f>+B8-B14</f>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="1">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="1">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="1">
-        <f>+SUM(B19:B20)</f>
-        <v>125000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="1">
-        <v>-10000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="E40" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="1">
-        <f>+SUM(B24:B26)</f>
-        <v>-2000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+    </row>
+    <row r="41" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="15">
+        <f>+B34/B6</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="1">
-        <f>+B16-B21+B27</f>
-        <v>173000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="1">
-        <v>-40000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="1">
-        <f>+SUM(B29:B30)</f>
-        <v>133000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="42" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="15">
+        <f>+B34/'Balance sheet'!B23</f>
+        <v>0.85806451612903223</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="4"/>
+      <c r="AF42" s="4"/>
+      <c r="AG42" s="4"/>
+      <c r="AH42" s="4"/>
+      <c r="AI42" s="4"/>
+      <c r="AJ42" s="4"/>
+    </row>
+    <row r="43" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="15">
+        <f>+B31/('Balance sheet'!B9-'Balance sheet'!B15)</f>
+        <v>0.61785714285714288</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="4"/>
+      <c r="AE43" s="4"/>
+      <c r="AF43" s="4"/>
+      <c r="AG43" s="4"/>
+      <c r="AH43" s="4"/>
+      <c r="AI43" s="4"/>
+      <c r="AJ43" s="4"/>
+    </row>
+    <row r="44" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="B44" s="15">
+        <f>+B34/'Balance sheet'!B9</f>
+        <v>0.42903225806451611</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E37" s="4" t="s">
+    </row>
+    <row r="45" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>133</v>
+    </row>
+    <row r="46" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" s="15">
+        <f>+B31/ABS(B27)</f>
+        <v>17.3</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7577,7 +7723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -7591,7 +7737,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>11</v>
@@ -7607,17 +7753,17 @@
     </row>
     <row r="3" spans="1:5" ht="103.5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B6" s="1">
         <v>100000</v>
@@ -7625,12 +7771,12 @@
     </row>
     <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B9" s="1">
         <v>50000</v>
@@ -7638,7 +7784,7 @@
     </row>
     <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B10" s="1">
         <v>-20000</v>
@@ -7646,7 +7792,7 @@
     </row>
     <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B11" s="1">
         <v>10000</v>
@@ -7654,7 +7800,7 @@
     </row>
     <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B12" s="1">
         <v>15000</v>
@@ -7662,7 +7808,7 @@
     </row>
     <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B13" s="1">
         <f>+SUM(B9:B12,B6)</f>
@@ -7671,12 +7817,12 @@
     </row>
     <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B16" s="1">
         <v>-75000</v>
@@ -7684,7 +7830,7 @@
     </row>
     <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B17" s="1">
         <f>+SUM(B16)</f>
@@ -7693,12 +7839,12 @@
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B20" s="1">
         <v>50000</v>
@@ -7706,7 +7852,7 @@
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B21" s="1">
         <v>-20000</v>
@@ -7714,7 +7860,7 @@
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B22" s="1">
         <v>-10000</v>
@@ -7722,7 +7868,7 @@
     </row>
     <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B23" s="1">
         <f>+SUM(B20:B22)</f>
@@ -7731,7 +7877,7 @@
     </row>
     <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B25" s="1">
         <v>100000</v>
@@ -7739,7 +7885,7 @@
     </row>
     <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B27" s="1">
         <v>500000</v>
@@ -7747,7 +7893,7 @@
     </row>
     <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B29" s="1">
         <f>+SUM(B25,B27)</f>
@@ -7763,8 +7909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7775,17 +7921,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
@@ -7793,27 +7939,27 @@
     </row>
     <row r="6" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
@@ -7821,17 +7967,17 @@
     </row>
     <row r="13" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="86.25" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
@@ -7839,22 +7985,22 @@
     </row>
     <row r="18" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
18-05-2023 Make .. continue
</commit_message>
<xml_diff>
--- a/financial_knwoledge/financial_statment.xlsx
+++ b/financial_knwoledge/financial_statment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\etc\financial_knwoledge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\suraj\etc\etc\financial_knwoledge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="financial statment" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Cash Flow statement" sheetId="6" r:id="rId4"/>
     <sheet name="Turnover ratio" sheetId="3" r:id="rId5"/>
     <sheet name="Ratio" sheetId="7" r:id="rId6"/>
+    <sheet name="Arti_industries-financial " sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="351">
   <si>
     <t>Financial statement</t>
   </si>
@@ -627,21 +628,486 @@
   </si>
   <si>
     <t>Solvency Ratio = Net Income / Long-Term Debt</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>AMOUNT (RS. IN LAKHS)</t>
+  </si>
+  <si>
+    <t>Revenue from operations</t>
+  </si>
+  <si>
+    <t>Other income</t>
+  </si>
+  <si>
+    <t>Total income</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>(a) Cost of materials consumed</t>
+  </si>
+  <si>
+    <t>(b) Cost of materials consumed</t>
+  </si>
+  <si>
+    <t>(c) Changes in inventories of finished goods, work-in-progress and stock-in-trade</t>
+  </si>
+  <si>
+    <t>(d) Employee benefits expense</t>
+  </si>
+  <si>
+    <t>(e) Finance costs</t>
+  </si>
+  <si>
+    <t>(f) Depreciation and amortisation expense</t>
+  </si>
+  <si>
+    <t>(g) Other expenses</t>
+  </si>
+  <si>
+    <t>Total Expenses</t>
+  </si>
+  <si>
+    <t>Profit/(Loss) before exceptional items and tax</t>
+  </si>
+  <si>
+    <t>Exceptional items</t>
+  </si>
+  <si>
+    <t>Tax Expenses</t>
+  </si>
+  <si>
+    <t>Current Tax</t>
+  </si>
+  <si>
+    <t>Deferred Tax</t>
+  </si>
+  <si>
+    <t>Total Tax expense</t>
+  </si>
+  <si>
+    <t>Net movement in regulatory deferral account balances related to profit or loss and the related deferred tax movement</t>
+  </si>
+  <si>
+    <t>Profit (Loss) for the period from continuing operations</t>
+  </si>
+  <si>
+    <t>Profit/(loss) from discontinued operations</t>
+  </si>
+  <si>
+    <t>Tax expense of discontinued operations</t>
+  </si>
+  <si>
+    <t>Profit/(loss) from Discontinued operations (after tax)</t>
+  </si>
+  <si>
+    <t>Profit/(loss) for the period</t>
+  </si>
+  <si>
+    <t>Share of profit/(loss) of associates</t>
+  </si>
+  <si>
+    <t>Consolidated Net Profit/Loss for the period</t>
+  </si>
+  <si>
+    <t>Other comprehensive income</t>
+  </si>
+  <si>
+    <t>Total comprehensive income</t>
+  </si>
+  <si>
+    <t>Total profit or loss, attributable to</t>
+  </si>
+  <si>
+    <t>Profit or loss, attributable to owners of parent</t>
+  </si>
+  <si>
+    <t>Total profit or loss, attributable to non-controlling interests</t>
+  </si>
+  <si>
+    <t>Total Comprehensive income for the period attributable to</t>
+  </si>
+  <si>
+    <t>Comprehensive income for the period attributable to owners of parent</t>
+  </si>
+  <si>
+    <t>Total comprehensive income for the period attributable to owners of parent non-controlling interests</t>
+  </si>
+  <si>
+    <t>Details of equity share capital</t>
+  </si>
+  <si>
+    <t>Paid-up equity share capital</t>
+  </si>
+  <si>
+    <t>Face Value (in Rs.)</t>
+  </si>
+  <si>
+    <t>Details of debt securities</t>
+  </si>
+  <si>
+    <t>Paid-up debt capital</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Face value of debt securities (in Rs.)</t>
+  </si>
+  <si>
+    <t>Reserve excluding Revaluation Reserves as per balance sheet of previous accounting year</t>
+  </si>
+  <si>
+    <t>Debenture redemption reserve</t>
+  </si>
+  <si>
+    <t>Earnings per share</t>
+  </si>
+  <si>
+    <t>Earnings per equity share for continuing operations</t>
+  </si>
+  <si>
+    <t>Basic EPS for continuing operations</t>
+  </si>
+  <si>
+    <t>Diluted EPS for continuing operations</t>
+  </si>
+  <si>
+    <t>Earnings per equity share for discontinued operations</t>
+  </si>
+  <si>
+    <t>Basic EPS for continued and discontinued operations</t>
+  </si>
+  <si>
+    <t>Diluted EPS for discontinued operations</t>
+  </si>
+  <si>
+    <t>Earnings per equity share</t>
+  </si>
+  <si>
+    <t>Diluted EPS for continued and discontinued operations</t>
+  </si>
+  <si>
+    <t>Debt equity ratio (in %)</t>
+  </si>
+  <si>
+    <t>Debt service coverage ratio (in %)</t>
+  </si>
+  <si>
+    <t>Interest service coverage ratio (in %)</t>
+  </si>
+  <si>
+    <t>Disclosure of notes on financial results by banks</t>
+  </si>
+  <si>
+    <t>AMOUNT (RS. IN Crores)</t>
+  </si>
+  <si>
+    <t>INCOME STATEMENT</t>
+  </si>
+  <si>
+    <t>BALANCE SHEET</t>
+  </si>
+  <si>
+    <t>(a)Property, Plant and Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(i)Investments </t>
+  </si>
+  <si>
+    <t>(a)Investment in Subsidiary &amp; Joint Control</t>
+  </si>
+  <si>
+    <t>(ii)Investments (Others )</t>
+  </si>
+  <si>
+    <t>(b)Other Financial Assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(h)Other Non-Current Assets </t>
+  </si>
+  <si>
+    <t>(a) Inventories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b) Financial Assets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(i) Investments </t>
+  </si>
+  <si>
+    <t>(i) Trade Receivables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ii) Cash and Cash Equivalents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(iii) Bank Balance Other than (ii) above </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(iv) Loans </t>
+  </si>
+  <si>
+    <t>(v) Other Current Finanical Assets</t>
+  </si>
+  <si>
+    <t>(c) Other Current Assets</t>
+  </si>
+  <si>
+    <t>Total Non-Current Assets</t>
+  </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>TOTAL ASSETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Current Liabilities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a) Financial Liabilities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Non-Current Assets. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Current Assets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part A ASSETS </t>
+  </si>
+  <si>
+    <t>Part B EQUITY AND LIBILITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Equity </t>
+  </si>
+  <si>
+    <t>(a) Equity Share Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b) Equity Share Capital pending allotment </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (c) Other Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Liabilities </t>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(i) Borrowings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(i) Lease Liabilities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ii) Provisions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b) Deferred Tax Liabilities </t>
+  </si>
+  <si>
+    <t>(c) Other Non-Current Liabilities</t>
+  </si>
+  <si>
+    <t>Total Non-Current Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (d) Non Controlling Interest </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Liabilities </t>
+  </si>
+  <si>
+    <t>(i) Borrowings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(i) Trade Payables due to - Micro and Small Entereprises </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other Than Micro and Small Entereprises</t>
+  </si>
+  <si>
+    <t>(iii) Others Financial Liabilities</t>
+  </si>
+  <si>
+    <t>(b) Provisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(c) Current Tax Liabilities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(d) Others Tax Liabilities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Current  Liabilities </t>
+  </si>
+  <si>
+    <t>Total EQUITY AND LIBILITIES</t>
+  </si>
+  <si>
+    <t>(b) Capital work-in-progress</t>
+  </si>
+  <si>
+    <t>(c)Right to use Assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(d)Goodwill </t>
+  </si>
+  <si>
+    <t>(e)Other intangible assets</t>
+  </si>
+  <si>
+    <t>(f)Intangible assets under Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(g)Financial Assets </t>
+  </si>
+  <si>
+    <t>Part A Cash Flow from Operating Activities:</t>
+  </si>
+  <si>
+    <t>Net Profit before Tax and Exceptional/Extraordinary Items</t>
+  </si>
+  <si>
+    <t>Adjustments for:</t>
+  </si>
+  <si>
+    <t>Finance Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustments for: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depreciation and Amortisation Expenses </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividend Income </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profit on Sale of Assets/Investments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidated Adjustment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating Profit before Working Capital Changes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Increase)/Decrease in Inventories </t>
+  </si>
+  <si>
+    <t>(Increase)/Decrease in Trade and Other Receivables</t>
+  </si>
+  <si>
+    <t>Increase/(Decrease) in Trade Payables and Other Current Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash Generated from Operations </t>
+  </si>
+  <si>
+    <t>Direct Taxes Paid</t>
+  </si>
+  <si>
+    <t>Net Cash Flow from Operating Activities(A)</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part B Cash Flow from Investing Activities: </t>
+  </si>
+  <si>
+    <t>Addition to Property, Plant &amp; Equipment/Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Increase)/Decrease in Other Investments </t>
+  </si>
+  <si>
+    <t>Dividend &amp; Interest Income from Subsidiary Companies</t>
+  </si>
+  <si>
+    <t>Interest income</t>
+  </si>
+  <si>
+    <t>Profit on Sale of Assets/Investments</t>
+  </si>
+  <si>
+    <t>Net Cash Flow from Investing Activities (B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part C Cash Flow from Financing Activities: </t>
+  </si>
+  <si>
+    <t>Proceeds/(Repayment) of Borrowings</t>
+  </si>
+  <si>
+    <t>Dividend Paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Cash Flow from Financing Activities (C) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash and Cash Equivalents (Opening Balance) </t>
+  </si>
+  <si>
+    <t>Cash and Cash Equivalents (Closing Balance)</t>
+  </si>
+  <si>
+    <t>CASH FLOW STATEMENT</t>
+  </si>
+  <si>
+    <t>Net Increase/(Decrease) in Cash and Cash Equivalents (A+B+C)</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Profit/(Loss) before tax(1-2)</t>
+  </si>
+  <si>
+    <t>Part 1 Revenue from operations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -728,16 +1194,74 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF5C5C5C"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5C5C5C"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3A2D7D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -745,58 +1269,156 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1115,7 +1737,7 @@
   <dimension ref="A1:AJ159"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7359,8 +7981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8122,8 +8744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8300,4 +8922,1547 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="19.5" thickBot="1">
+      <c r="A1" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="E1" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="I1" s="35" t="s">
+        <v>346</v>
+      </c>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A2" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A3" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="E3" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="27">
+        <v>194523</v>
+      </c>
+      <c r="C4">
+        <f>+B4/100</f>
+        <v>1945.23</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="J4" s="32">
+        <v>26077</v>
+      </c>
+      <c r="K4">
+        <f>+J4/100</f>
+        <v>260.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="28">
+        <v>232</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C56" si="0">+B5/100</f>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="30">
+        <v>92274</v>
+      </c>
+      <c r="G5">
+        <f>+F5/100</f>
+        <v>922.74</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="21.75" thickBot="1">
+      <c r="A6" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="27">
+        <f>+SUM(B4:B5)</f>
+        <v>194755</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1947.55</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="F6" s="30">
+        <v>6220</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G62" si="1">+F6/100</f>
+        <v>62.2</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="J6">
+        <v>2105</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K11" si="2">+J6/100</f>
+        <v>21.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A7" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="E7" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7">
+        <v>114</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="J7">
+        <v>6254</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>62.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A8" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="27">
+        <v>101430</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1014.3</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8">
+        <v>178</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1.78</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="J8">
+        <v>-128</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>-1.28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="27">
+        <v>28082</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>280.82</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9">
+        <v>-94</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>-0.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="27">
+        <v>-12536</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-125.36</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F10">
+        <v>3967</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>39.67</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="J10">
+        <v>45</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A11" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="27">
+        <v>12969</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>129.69</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="J11" s="32">
+        <f>+SUM(J4:J10)</f>
+        <v>34259</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>342.59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A12" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="27">
+        <v>2105</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>21.05</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A13" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="27">
+        <v>6254</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>62.54</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="J13">
+        <v>-12666</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13:K18" si="3">+J13/100</f>
+        <v>-126.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A14" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="27">
+        <v>30374</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>303.74</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="F14">
+        <v>3552</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>35.520000000000003</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="J14">
+        <v>-2076</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>-20.76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="21.75" thickBot="1">
+      <c r="A15" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="27">
+        <f>+SUM(B8:B14)</f>
+        <v>168678</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1686.78</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F15">
+        <v>944</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>9.44</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="J15">
+        <v>13021</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>130.21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A16" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="27">
+        <v>26077</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>260.77</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="F16">
+        <v>249</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="J16" s="32">
+        <f>+SUM(J11:J15)</f>
+        <v>32538</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>325.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A17" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" s="28">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="F17" s="30">
+        <f>+SUM(F5:F16)</f>
+        <v>107516</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1075.1600000000001</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="J17">
+        <v>-6238</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>-62.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A18" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B18" s="27">
+        <f>+SUM(B6-B15)</f>
+        <v>26077</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>260.77</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="J18" s="32">
+        <f>+SUM(J16,J17)</f>
+        <v>26300</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A19" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="E19" s="26" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A20" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="27">
+        <v>5912</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>59.12</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="F20">
+        <v>60204</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>602.04</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A21" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="28">
+        <v>816</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>8.16</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="J21">
+        <v>-11966</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K26" si="4">+J21/100</f>
+        <v>-119.66</v>
+      </c>
+      <c r="O21" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A22" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" s="27">
+        <v>6728</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>67.28</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="F22">
+        <v>3818</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>38.18</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="J22">
+        <v>-3868</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>-38.68</v>
+      </c>
+      <c r="O22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A23" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" s="28">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="F23">
+        <v>44005</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>440.05</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A24" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="27">
+        <v>19349</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>193.49</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="F24">
+        <v>2493</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>24.93</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="J24">
+        <v>94</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A25" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" s="28">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="J25">
+        <v>-45</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A26" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="28">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="F26">
+        <v>710</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>7.1</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="J26">
+        <f>+SUM(J21:J25)</f>
+        <v>-15781</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>-157.81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A27" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B27" s="28">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="F27">
+        <v>3581</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>35.81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A28" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="27">
+        <v>19349</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>193.49</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="F28">
+        <v>758</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>7.58</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A29" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="28">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="F29">
+        <f>+SUM(F20:F28)</f>
+        <v>115576</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1155.76</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="J29">
+        <v>-12429</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K32" si="5">+J29/100</f>
+        <v>-124.29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A30" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" s="27">
+        <v>19349</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>193.49</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="F30" s="30">
+        <f>+SUM(F17,F29)</f>
+        <v>223092</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>2230.92</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="J30">
+        <v>-2105</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="5"/>
+        <v>-21.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A31" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B31" s="28">
+        <v>-345</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>-3.45</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="J31">
+        <v>-1813</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="5"/>
+        <v>-18.13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A32" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" s="27">
+        <v>19004</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>190.04</v>
+      </c>
+      <c r="I32" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="J32">
+        <f>+SUM(J29:J31)</f>
+        <v>-16347</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>-163.47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A33" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="E33" s="26" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A34" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B34" s="27">
+        <v>19349</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>193.49</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="J34" s="32">
+        <f>+SUM(J18,J26,J32)</f>
+        <v>-5828</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ref="K34:K36" si="6">+J34/100</f>
+        <v>-58.28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A35" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B35" s="28">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="F35">
+        <v>4532</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>45.32</v>
+      </c>
+      <c r="I35" t="s">
+        <v>344</v>
+      </c>
+      <c r="J35">
+        <v>8327</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>83.27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A36" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B36" s="37"/>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>345</v>
+      </c>
+      <c r="J36" s="32">
+        <f>+SUM(J34,J35)</f>
+        <v>2499</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="6"/>
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="75" customHeight="1" thickBot="1">
+      <c r="A37" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B37" s="27">
+        <v>19004</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>190.04</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F37">
+        <v>151317</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>1513.17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A38" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="B38" s="28">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="21.75" thickBot="1">
+      <c r="A39" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="F39">
+        <f>+SUM(F35:F37)</f>
+        <v>155849</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1558.49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A40" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="B40" s="27">
+        <v>4531.3</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>45.313000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A41" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" s="28">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A42" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="B42" s="37"/>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A43" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="B43" s="28"/>
+      <c r="E43" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A44" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" s="28"/>
+      <c r="E44" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="F44">
+        <v>18</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A45" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="27">
+        <v>151317</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>1513.17</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="F45">
+        <v>53</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A46" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46">
+        <v>132</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A47" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="F47">
+        <v>7884</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>78.84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A48" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="60" customHeight="1" thickBot="1">
+      <c r="A49" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="B49" s="28">
+        <v>21.35</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0.21350000000000002</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="F49">
+        <f>+SUM(F42:F48)</f>
+        <v>8087</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>80.87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A50" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B50" s="28">
+        <v>21.35</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>0.21350000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A51" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="B51" s="37"/>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="60" customHeight="1" thickBot="1">
+      <c r="A52" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B52" s="28">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A53" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B53" s="28">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="F53">
+        <v>21378</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>213.78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A54" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="B54" s="37"/>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F54">
+        <v>1265</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>12.65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="A55" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55" s="28">
+        <v>21.35</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>0.21350000000000002</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="F55">
+        <v>33410</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>334.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A56" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B56" s="28">
+        <v>21.35</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>0.21350000000000002</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="F56">
+        <v>1692</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>16.920000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A57" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B57" s="28"/>
+      <c r="E57" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="F57">
+        <v>1121</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>11.21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A58" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="B58" s="28"/>
+      <c r="E58" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F58">
+        <v>290</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A59" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" s="28"/>
+      <c r="E59" s="26" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="21.75" thickBot="1">
+      <c r="A60" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="B60" s="28"/>
+      <c r="E60" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="F60">
+        <f>+SUM(F53:F58)</f>
+        <v>59156</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>591.55999999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="21">
+      <c r="E62" s="31" t="s">
+        <v>309</v>
+      </c>
+      <c r="F62">
+        <f>+SUM(F39,F49,F60)</f>
+        <v>223092</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>2230.92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="38" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="E64" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="I64" s="33" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17.25">
+      <c r="A65" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="39">
+        <f>+(C4-C15)/C4</f>
+        <v>0.13286346601687207</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17.25">
+      <c r="A66" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="4">
+        <f>+C16</f>
+        <v>260.77</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17.25">
+      <c r="A67" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17.25">
+      <c r="A68" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17.25">
+      <c r="A69" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17.25">
+      <c r="A70" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17.25">
+      <c r="A71" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17.25">
+      <c r="A72" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17.25">
+      <c r="A73" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4">
+      <c r="D95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4">
+      <c r="D99" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4">
+      <c r="D101" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finacial knowlogde -- continue 19-05-2023
</commit_message>
<xml_diff>
--- a/financial_knwoledge/financial_statment.xlsx
+++ b/financial_knwoledge/financial_statment.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="340">
   <si>
     <t>Financial statement</t>
   </si>
@@ -642,9 +642,6 @@
     <t>Other income</t>
   </si>
   <si>
-    <t>Total income</t>
-  </si>
-  <si>
     <t>Expenses</t>
   </si>
   <si>
@@ -669,18 +666,6 @@
     <t>(g) Other expenses</t>
   </si>
   <si>
-    <t>Total Expenses</t>
-  </si>
-  <si>
-    <t>Profit/(Loss) before exceptional items and tax</t>
-  </si>
-  <si>
-    <t>Exceptional items</t>
-  </si>
-  <si>
-    <t>Tax Expenses</t>
-  </si>
-  <si>
     <t>Current Tax</t>
   </si>
   <si>
@@ -690,54 +675,15 @@
     <t>Total Tax expense</t>
   </si>
   <si>
-    <t>Net movement in regulatory deferral account balances related to profit or loss and the related deferred tax movement</t>
-  </si>
-  <si>
-    <t>Profit (Loss) for the period from continuing operations</t>
-  </si>
-  <si>
-    <t>Profit/(loss) from discontinued operations</t>
-  </si>
-  <si>
-    <t>Tax expense of discontinued operations</t>
-  </si>
-  <si>
-    <t>Profit/(loss) from Discontinued operations (after tax)</t>
-  </si>
-  <si>
-    <t>Profit/(loss) for the period</t>
-  </si>
-  <si>
-    <t>Share of profit/(loss) of associates</t>
-  </si>
-  <si>
-    <t>Consolidated Net Profit/Loss for the period</t>
-  </si>
-  <si>
-    <t>Other comprehensive income</t>
-  </si>
-  <si>
-    <t>Total comprehensive income</t>
-  </si>
-  <si>
-    <t>Total profit or loss, attributable to</t>
-  </si>
-  <si>
     <t>Profit or loss, attributable to owners of parent</t>
   </si>
   <si>
-    <t>Total profit or loss, attributable to non-controlling interests</t>
-  </si>
-  <si>
     <t>Total Comprehensive income for the period attributable to</t>
   </si>
   <si>
     <t>Comprehensive income for the period attributable to owners of parent</t>
   </si>
   <si>
-    <t>Total comprehensive income for the period attributable to owners of parent non-controlling interests</t>
-  </si>
-  <si>
     <t>Details of equity share capital</t>
   </si>
   <si>
@@ -786,24 +732,6 @@
     <t>Diluted EPS for discontinued operations</t>
   </si>
   <si>
-    <t>Earnings per equity share</t>
-  </si>
-  <si>
-    <t>Diluted EPS for continued and discontinued operations</t>
-  </si>
-  <si>
-    <t>Debt equity ratio (in %)</t>
-  </si>
-  <si>
-    <t>Debt service coverage ratio (in %)</t>
-  </si>
-  <si>
-    <t>Interest service coverage ratio (in %)</t>
-  </si>
-  <si>
-    <t>Disclosure of notes on financial results by banks</t>
-  </si>
-  <si>
     <t>AMOUNT (RS. IN Crores)</t>
   </si>
   <si>
@@ -1074,10 +1002,49 @@
     <t>Ratio</t>
   </si>
   <si>
-    <t>Profit/(Loss) before tax(1-2)</t>
-  </si>
-  <si>
     <t>Part 1 Revenue from operations</t>
+  </si>
+  <si>
+    <t>No of outstanding shares(in lac)</t>
+  </si>
+  <si>
+    <t>Earlier year tax</t>
+  </si>
+  <si>
+    <t>(1)Total income</t>
+  </si>
+  <si>
+    <t>(2)Total Expenses</t>
+  </si>
+  <si>
+    <t>(3)Profit/(Loss) before exceptional items and tax(1-2)</t>
+  </si>
+  <si>
+    <t>(4)Exceptional items</t>
+  </si>
+  <si>
+    <t>(5)Profit/(Loss) before tax(3-4)</t>
+  </si>
+  <si>
+    <t>(6)Tax Expenses</t>
+  </si>
+  <si>
+    <t>Net profit /loss for a period(7-8)</t>
+  </si>
+  <si>
+    <t>(7)Net profit /loss from ordinary activity after tax(5-6)</t>
+  </si>
+  <si>
+    <t>(8)exceptional item</t>
+  </si>
+  <si>
+    <t>Non Controlling interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTHER COMPREHENSIVE INCOME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item that will be reclacified </t>
   </si>
 </sst>
 </file>
@@ -1086,14 +1053,21 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1337,88 +1311,89 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8929,12 +8904,12 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="68" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
@@ -8946,21 +8921,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="35" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="E1" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="I1" s="35" t="s">
-        <v>346</v>
-      </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="A1" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="E1" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="I1" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="25" t="s">
@@ -8970,7 +8945,7 @@
         <v>202</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>201</v>
@@ -8979,7 +8954,7 @@
         <v>202</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>201</v>
@@ -8988,19 +8963,19 @@
         <v>202</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="36" t="s">
-        <v>350</v>
-      </c>
-      <c r="B3" s="37"/>
+      <c r="A3" s="37" t="s">
+        <v>325</v>
+      </c>
+      <c r="B3" s="38"/>
       <c r="E3" s="29" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1">
@@ -9015,10 +8990,10 @@
         <v>1945.23</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="J4" s="32">
         <v>26077</v>
@@ -9036,11 +9011,11 @@
         <v>232</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C56" si="0">+B5/100</f>
+        <f t="shared" ref="C5:C40" si="0">+B5/100</f>
         <v>2.3199999999999998</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="F5" s="30">
         <v>92274</v>
@@ -9050,12 +9025,12 @@
         <v>922.74</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21.75" thickBot="1">
       <c r="A6" s="31" t="s">
-        <v>205</v>
+        <v>328</v>
       </c>
       <c r="B6" s="27">
         <f>+SUM(B4:B5)</f>
@@ -9066,7 +9041,7 @@
         <v>1947.55</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="F6" s="30">
         <v>6220</v>
@@ -9076,7 +9051,7 @@
         <v>62.2</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="J6">
         <v>2105</v>
@@ -9087,12 +9062,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A7" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="B7" s="37"/>
+      <c r="A7" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="38"/>
       <c r="E7" s="26" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="F7">
         <v>114</v>
@@ -9102,7 +9077,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="J7">
         <v>6254</v>
@@ -9114,7 +9089,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1">
       <c r="A8" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B8" s="27">
         <v>101430</v>
@@ -9124,7 +9099,7 @@
         <v>1014.3</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="F8">
         <v>178</v>
@@ -9134,7 +9109,7 @@
         <v>1.78</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="J8">
         <v>-128</v>
@@ -9146,7 +9121,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="27">
         <v>28082</v>
@@ -9156,7 +9131,7 @@
         <v>280.82</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="F9">
         <v>18</v>
@@ -9166,7 +9141,7 @@
         <v>0.18</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="J9">
         <v>-94</v>
@@ -9178,7 +9153,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="27">
         <v>-12536</v>
@@ -9188,7 +9163,7 @@
         <v>-125.36</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="F10">
         <v>3967</v>
@@ -9198,7 +9173,7 @@
         <v>39.67</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="J10">
         <v>45</v>
@@ -9210,7 +9185,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1">
       <c r="A11" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" s="27">
         <v>12969</v>
@@ -9220,10 +9195,10 @@
         <v>129.69</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="J11" s="32">
         <f>+SUM(J4:J10)</f>
@@ -9236,7 +9211,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1">
       <c r="A12" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="27">
         <v>2105</v>
@@ -9246,15 +9221,15 @@
         <v>21.05</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1">
       <c r="A13" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="27">
         <v>6254</v>
@@ -9264,10 +9239,10 @@
         <v>62.54</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="J13">
         <v>-12666</v>
@@ -9279,7 +9254,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14" s="27">
         <v>30374</v>
@@ -9289,7 +9264,7 @@
         <v>303.74</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="F14">
         <v>3552</v>
@@ -9299,7 +9274,7 @@
         <v>35.520000000000003</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="J14">
         <v>-2076</v>
@@ -9311,7 +9286,7 @@
     </row>
     <row r="15" spans="1:11" ht="21.75" thickBot="1">
       <c r="A15" s="31" t="s">
-        <v>214</v>
+        <v>329</v>
       </c>
       <c r="B15" s="27">
         <f>+SUM(B8:B14)</f>
@@ -9322,7 +9297,7 @@
         <v>1686.78</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="F15">
         <v>944</v>
@@ -9332,7 +9307,7 @@
         <v>9.44</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="J15">
         <v>13021</v>
@@ -9342,11 +9317,12 @@
         <v>130.21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A16" s="26" t="s">
-        <v>215</v>
+    <row r="16" spans="1:11" ht="21.75" thickBot="1">
+      <c r="A16" s="31" t="s">
+        <v>330</v>
       </c>
       <c r="B16" s="27">
+        <f>+B6-B15</f>
         <v>26077</v>
       </c>
       <c r="C16">
@@ -9354,7 +9330,7 @@
         <v>260.77</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="F16">
         <v>249</v>
@@ -9364,7 +9340,7 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="I16" s="33" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="J16" s="32">
         <f>+SUM(J11:J15)</f>
@@ -9376,8 +9352,8 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="21.75" thickBot="1">
-      <c r="A17" s="26" t="s">
-        <v>216</v>
+      <c r="A17" s="31" t="s">
+        <v>331</v>
       </c>
       <c r="B17" s="28">
         <v>0</v>
@@ -9387,7 +9363,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="F17" s="30">
         <f>+SUM(F5:F16)</f>
@@ -9398,7 +9374,7 @@
         <v>1075.1600000000001</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="J17">
         <v>-6238</v>
@@ -9410,7 +9386,7 @@
     </row>
     <row r="18" spans="1:15" ht="21.75" thickBot="1">
       <c r="A18" s="31" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="B18" s="27">
         <f>+SUM(B6-B15)</f>
@@ -9421,7 +9397,7 @@
         <v>260.77</v>
       </c>
       <c r="I18" s="33" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="J18" s="32">
         <f>+SUM(J16,J17)</f>
@@ -9432,28 +9408,28 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A19" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="B19" s="37"/>
+    <row r="19" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A19" s="31" t="s">
+        <v>333</v>
+      </c>
+      <c r="B19" s="31"/>
       <c r="E19" s="26" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1">
       <c r="A20" s="26" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B20" s="27">
-        <v>5912</v>
+        <v>5599</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>59.12</v>
+        <v>55.99</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="F20">
         <v>60204</v>
@@ -9463,25 +9439,25 @@
         <v>602.04</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1">
       <c r="A21" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B21" s="28">
-        <v>816</v>
+        <v>327</v>
+      </c>
+      <c r="B21" s="27">
+        <v>313</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>8.16</v>
+        <v>3.13</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="J21">
         <v>-11966</v>
@@ -9491,22 +9467,22 @@
         <v>-119.66</v>
       </c>
       <c r="O21" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1">
       <c r="A22" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B22" s="27">
-        <v>6728</v>
+        <v>214</v>
+      </c>
+      <c r="B22" s="28">
+        <v>817</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>67.28</v>
+        <v>8.17</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="F22">
         <v>3818</v>
@@ -9516,7 +9492,7 @@
         <v>38.18</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="J22">
         <v>-3868</v>
@@ -9526,22 +9502,23 @@
         <v>-38.68</v>
       </c>
       <c r="O22" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A23" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="B23" s="28">
-        <v>0</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A23" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="27">
+        <f>+SUM(B20:B22)</f>
+        <v>6729</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67.290000000000006</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="F23">
         <v>44005</v>
@@ -9551,7 +9528,7 @@
         <v>440.05</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="J23">
         <v>4</v>
@@ -9561,19 +9538,20 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A24" s="26" t="s">
-        <v>222</v>
+    <row r="24" spans="1:15" ht="21.75" thickBot="1">
+      <c r="A24" s="31" t="s">
+        <v>335</v>
       </c>
       <c r="B24" s="27">
-        <v>19349</v>
+        <f>+B18-B23</f>
+        <v>19348</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>193.49</v>
+        <v>193.48</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="F24">
         <v>2493</v>
@@ -9583,7 +9561,7 @@
         <v>24.93</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="J24">
         <v>94</v>
@@ -9594,10 +9572,10 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A25" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="B25" s="28">
+      <c r="A25" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="B25" s="27">
         <v>0</v>
       </c>
       <c r="C25">
@@ -9605,7 +9583,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="F25">
         <v>7</v>
@@ -9615,7 +9593,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="J25">
         <v>-45</v>
@@ -9627,17 +9605,18 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1">
       <c r="A26" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="B26" s="28">
-        <v>0</v>
+        <v>334</v>
+      </c>
+      <c r="B26" s="27">
+        <f>+B24-B25</f>
+        <v>19348</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>193.48</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="F26">
         <v>710</v>
@@ -9647,7 +9626,7 @@
         <v>7.1</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="J26">
         <f>+SUM(J21:J25)</f>
@@ -9660,17 +9639,18 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1">
       <c r="A27" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="B27" s="28">
-        <v>0</v>
+        <v>216</v>
+      </c>
+      <c r="B27" s="27">
+        <f>+B26</f>
+        <v>19348</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>193.48</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="F27">
         <v>3581</v>
@@ -9682,17 +9662,17 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1">
       <c r="A28" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B28" s="27">
-        <v>19349</v>
+        <v>337</v>
+      </c>
+      <c r="B28" s="28">
+        <v>0</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>193.49</v>
+        <v>0</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="F28">
         <v>758</v>
@@ -9702,22 +9682,20 @@
         <v>7.58</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="21.75" thickBot="1">
       <c r="A29" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="B29" s="28">
-        <v>0</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="B29" s="27"/>
       <c r="C29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="F29">
         <f>+SUM(F20:F28)</f>
@@ -9728,7 +9706,7 @@
         <v>1155.76</v>
       </c>
       <c r="I29" s="26" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="J29">
         <v>-12429</v>
@@ -9740,17 +9718,17 @@
     </row>
     <row r="30" spans="1:15" ht="21.75" thickBot="1">
       <c r="A30" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30" s="27">
-        <v>19349</v>
+        <v>339</v>
+      </c>
+      <c r="B30" s="28">
+        <v>-345</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>193.49</v>
+        <v>-3.45</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="F30" s="30">
         <f>+SUM(F17,F29)</f>
@@ -9761,7 +9739,7 @@
         <v>2230.92</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="J30">
         <v>-2105</v>
@@ -9773,17 +9751,18 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1">
       <c r="A31" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="B31" s="28">
-        <v>-345</v>
+        <v>217</v>
+      </c>
+      <c r="B31" s="27">
+        <f>+SUM(B27,B28,B30)</f>
+        <v>19003</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>-3.45</v>
+        <v>190.03</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="J31">
         <v>-1813</v>
@@ -9794,18 +9773,14 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A32" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="B32" s="27">
-        <v>19004</v>
-      </c>
+      <c r="A32" s="26"/>
+      <c r="B32" s="28"/>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>190.04</v>
+        <v>0</v>
       </c>
       <c r="I32" s="33" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="J32">
         <f>+SUM(J29:J31)</f>
@@ -9817,30 +9792,32 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A33" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="B33" s="37"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E33" s="26" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A34" s="26" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B34" s="27">
-        <v>19349</v>
+        <v>19004</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>193.49</v>
+        <v>190.04</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="I34" s="34" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="J34" s="32">
         <f>+SUM(J18,J26,J32)</f>
@@ -9852,18 +9829,12 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A35" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="B35" s="28">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" s="38"/>
       <c r="E35" s="26" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="F35">
         <v>4532</v>
@@ -9873,7 +9844,7 @@
         <v>45.32</v>
       </c>
       <c r="I35" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="J35">
         <v>8327</v>
@@ -9884,16 +9855,18 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A36" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="B36" s="37"/>
+      <c r="A36" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" s="27">
+        <v>4531.3</v>
+      </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45.313000000000002</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -9903,7 +9876,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="J36" s="32">
         <f>+SUM(J34,J35)</f>
@@ -9916,17 +9889,17 @@
     </row>
     <row r="37" spans="1:11" ht="75" customHeight="1" thickBot="1">
       <c r="A37" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="B37" s="27">
-        <v>19004</v>
+        <v>221</v>
+      </c>
+      <c r="B37" s="28">
+        <v>5</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>190.04</v>
+        <v>0.05</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="F37">
         <v>151317</v>
@@ -9937,31 +9910,29 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A38" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B38" s="28">
-        <v>0</v>
-      </c>
+      <c r="A38" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="38"/>
       <c r="C38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21.75" thickBot="1">
-      <c r="A39" s="36" t="s">
-        <v>237</v>
-      </c>
-      <c r="B39" s="37"/>
+      <c r="A39" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" s="28"/>
       <c r="C39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="F39">
         <f>+SUM(F35:F37)</f>
@@ -9974,60 +9945,64 @@
     </row>
     <row r="40" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A40" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="B40" s="27">
-        <v>4531.3</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="B40" s="28"/>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>45.313000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1">
       <c r="A41" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="B41" s="28">
-        <v>5</v>
+        <v>226</v>
+      </c>
+      <c r="B41" s="27">
+        <v>151317</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f>+B36/100</f>
+        <v>45.313000000000002</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A42" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="C42">
+        <f>+B37/100</f>
         <v>0.05</v>
       </c>
-      <c r="E41" s="26" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A42" s="36" t="s">
-        <v>240</v>
-      </c>
-      <c r="B42" s="37"/>
-      <c r="C42">
-        <f t="shared" si="0"/>
+      <c r="E42" s="26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A43" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43">
+        <f>+B38/100</f>
         <v>0</v>
       </c>
-      <c r="E42" s="26" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="30" customHeight="1" thickBot="1">
-      <c r="A43" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="B43" s="28"/>
       <c r="E43" s="26" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A44" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="B44" s="28"/>
+      <c r="A44" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="38"/>
       <c r="E44" s="26" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="F44">
         <v>18</v>
@@ -10039,17 +10014,13 @@
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1">
       <c r="A45" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="B45" s="27">
-        <v>151317</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="0"/>
-        <v>1513.17</v>
+        <v>230</v>
+      </c>
+      <c r="B45" s="28">
+        <v>21.35</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="F45">
         <v>53</v>
@@ -10061,13 +10032,17 @@
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1">
       <c r="A46" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
+      </c>
+      <c r="B46" s="28">
+        <v>21.35</v>
+      </c>
+      <c r="C46">
+        <f>+B41/100</f>
+        <v>1513.17</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="F46">
         <v>132</v>
@@ -10078,16 +10053,12 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A47" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="B47" s="37"/>
-      <c r="C47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A47" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47" s="38"/>
       <c r="E47" s="26" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="F47">
         <v>7884</v>
@@ -10098,31 +10069,33 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="30" customHeight="1" thickBot="1">
-      <c r="A48" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="B48" s="37"/>
+      <c r="A48" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B48" s="28">
+        <v>0</v>
+      </c>
       <c r="C48">
-        <f t="shared" si="0"/>
+        <f>+B43/100</f>
         <v>0</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="60" customHeight="1" thickBot="1">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="21.75" thickBot="1">
       <c r="A49" s="26" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B49" s="28">
-        <v>21.35</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
-        <v>0.21350000000000002</v>
+        <f>+B44/100</f>
+        <v>0</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="F49">
         <f>+SUM(F42:F48)</f>
@@ -10133,59 +10106,23 @@
         <v>80.87</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A50" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="B50" s="28">
-        <v>21.35</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="0"/>
-        <v>0.21350000000000002</v>
-      </c>
-    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="51" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A51" s="36" t="s">
-        <v>250</v>
-      </c>
-      <c r="B51" s="37"/>
-      <c r="C51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="E51" s="26" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="60" customHeight="1" thickBot="1">
-      <c r="A52" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="B52" s="28">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A52" s="35" t="s">
+        <v>324</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A53" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="B53" s="28">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="E53" s="26" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="F53">
         <v>21378</v>
@@ -10196,16 +10133,8 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A54" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="B54" s="37"/>
-      <c r="C54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="E54" s="26" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="F54">
         <v>1265</v>
@@ -10216,18 +10145,8 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" customHeight="1" thickBot="1">
-      <c r="A55" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="B55" s="28">
-        <v>21.35</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="0"/>
-        <v>0.21350000000000002</v>
-      </c>
       <c r="E55" s="26" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="F55">
         <v>33410</v>
@@ -10238,18 +10157,8 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A56" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="B56" s="28">
-        <v>21.35</v>
-      </c>
-      <c r="C56">
-        <f t="shared" si="0"/>
-        <v>0.21350000000000002</v>
-      </c>
       <c r="E56" s="26" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="F56">
         <v>1692</v>
@@ -10260,12 +10169,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A57" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="B57" s="28"/>
       <c r="E57" s="26" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="F57">
         <v>1121</v>
@@ -10276,12 +10181,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A58" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="B58" s="28"/>
       <c r="E58" s="26" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="F58">
         <v>290</v>
@@ -10292,21 +10193,13 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A59" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="B59" s="28"/>
       <c r="E59" s="26" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="21.75" thickBot="1">
-      <c r="A60" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="B60" s="28"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="21">
       <c r="E60" s="31" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="F60">
         <f>+SUM(F53:F58)</f>
@@ -10319,7 +10212,7 @@
     </row>
     <row r="62" spans="1:9" ht="21">
       <c r="E62" s="31" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="F62">
         <f>+SUM(F39,F49,F60)</f>
@@ -10330,137 +10223,156 @@
         <v>2230.92</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="38" t="s">
-        <v>348</v>
-      </c>
-    </row>
     <row r="64" spans="1:9">
-      <c r="E64" s="38" t="s">
-        <v>348</v>
+      <c r="E64" s="35" t="s">
+        <v>324</v>
       </c>
       <c r="I64" s="33" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="17.25">
-      <c r="A65" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17.25">
+      <c r="A66" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B65" s="39">
+      <c r="B66" s="39">
         <f>+(C4-C15)/C4</f>
         <v>0.13286346601687207</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C66" s="19" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="17.25">
-      <c r="A66" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B66" s="4">
-        <f>+C16</f>
-        <v>260.77</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17.25">
       <c r="A67" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" s="4"/>
+        <v>117</v>
+      </c>
+      <c r="B67" s="39">
+        <f>+B18/B6</f>
+        <v>0.1338964339811558</v>
+      </c>
       <c r="C67" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17.25">
       <c r="A68" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" s="4"/>
+        <v>120</v>
+      </c>
+      <c r="B68" s="39">
+        <f>+B33/B6</f>
+        <v>0</v>
+      </c>
       <c r="C68" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17.25">
       <c r="A69" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B69" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="B69" s="39">
+        <f>+B31/F39</f>
+        <v>0.12193212660973121</v>
+      </c>
       <c r="C69" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17.25">
       <c r="A70" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B70" s="4"/>
+        <v>126</v>
+      </c>
+      <c r="B70" s="39">
+        <f>+B18/(F30-F49)</f>
+        <v>0.12128555149880235</v>
+      </c>
       <c r="C70" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17.25">
       <c r="A71" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" s="4"/>
+        <v>129</v>
+      </c>
+      <c r="B71" s="39">
+        <f>+B18/F30</f>
+        <v>0.11688899646782493</v>
+      </c>
       <c r="C71" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17.25">
       <c r="A72" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="39">
+        <f>+B18/A80</f>
+        <v>7.1936551724137932</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17.25">
+      <c r="A73" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4" t="s">
+      <c r="B73" s="39"/>
+      <c r="C73" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.25">
-      <c r="A73" s="15" t="s">
+    <row r="74" spans="1:3" ht="17.25">
+      <c r="A74" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4" t="s">
+      <c r="B74" s="39">
+        <f>+B18/B23</f>
+        <v>3.875315797295289</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="40" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>3625</v>
       </c>
     </row>
     <row r="95" spans="4:4">
       <c r="D95" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
     </row>
     <row r="99" spans="4:4">
       <c r="D99" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
     </row>
     <row r="101" spans="4:4">
       <c r="D101" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="10">
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A47:B47"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>